<commit_message>
Made a number of updates to the sisepuede sampling system and the models
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5004" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5007" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5009" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS15"/>
+  <dimension ref="A1:AS12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,12 +725,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>General</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>va_commercial_mmm_usd</t>
+          <t>area_gnrl_country_ha</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -742,123 +745,123 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>38.83107386</v>
+        <v>328726000</v>
       </c>
       <c r="K3" t="n">
-        <v>40.7395256</v>
+        <v>328726000</v>
       </c>
       <c r="L3" t="n">
-        <v>42.25398672</v>
+        <v>328726000</v>
       </c>
       <c r="M3" t="n">
-        <v>43.09221382</v>
+        <v>328726000</v>
       </c>
       <c r="N3" t="n">
-        <v>44.39106086</v>
+        <v>328726000</v>
       </c>
       <c r="O3" t="n">
-        <v>45.67741973</v>
+        <v>328726000</v>
       </c>
       <c r="P3" t="n">
-        <v>47.09170214</v>
+        <v>328726000</v>
       </c>
       <c r="Q3" t="n">
-        <v>48.59598329</v>
+        <v>328726000</v>
       </c>
       <c r="R3" t="n">
-        <v>50.25520448</v>
+        <v>328726000</v>
       </c>
       <c r="S3" t="n">
-        <v>52.07124644</v>
+        <v>328726000</v>
       </c>
       <c r="T3" t="n">
-        <v>53.95028727</v>
+        <v>328726000</v>
       </c>
       <c r="U3" t="n">
-        <v>55.89469218</v>
+        <v>328726000</v>
       </c>
       <c r="V3" t="n">
-        <v>57.90688651</v>
+        <v>328726000</v>
       </c>
       <c r="W3" t="n">
-        <v>59.98936838</v>
+        <v>328726000</v>
       </c>
       <c r="X3" t="n">
-        <v>62.14470074</v>
+        <v>328726000</v>
       </c>
       <c r="Y3" t="n">
-        <v>64.37550593</v>
+        <v>328726000</v>
       </c>
       <c r="Z3" t="n">
-        <v>66.68447044</v>
+        <v>328726000</v>
       </c>
       <c r="AA3" t="n">
-        <v>69.07436058</v>
+        <v>328726000</v>
       </c>
       <c r="AB3" t="n">
-        <v>71.54799061</v>
+        <v>328726000</v>
       </c>
       <c r="AC3" t="n">
-        <v>74.10827634</v>
+        <v>328726000</v>
       </c>
       <c r="AD3" t="n">
-        <v>76.75818214</v>
+        <v>328726000</v>
       </c>
       <c r="AE3" t="n">
-        <v>79.50074256000001</v>
+        <v>328726000</v>
       </c>
       <c r="AF3" t="n">
-        <v>82.33907012</v>
+        <v>328726000</v>
       </c>
       <c r="AG3" t="n">
-        <v>85.27635393</v>
+        <v>328726000</v>
       </c>
       <c r="AH3" t="n">
-        <v>88.3158834</v>
+        <v>328726000</v>
       </c>
       <c r="AI3" t="n">
-        <v>91.46103932</v>
+        <v>328726000</v>
       </c>
       <c r="AJ3" t="n">
-        <v>94.71529351</v>
+        <v>328726000</v>
       </c>
       <c r="AK3" t="n">
-        <v>98.08223058</v>
+        <v>328726000</v>
       </c>
       <c r="AL3" t="n">
-        <v>101.5655288</v>
+        <v>328726000</v>
       </c>
       <c r="AM3" t="n">
-        <v>105.1689578</v>
+        <v>328726000</v>
       </c>
       <c r="AN3" t="n">
-        <v>108.8964306</v>
+        <v>328726000</v>
       </c>
       <c r="AO3" t="n">
-        <v>112.7520034</v>
+        <v>328726000</v>
       </c>
       <c r="AP3" t="n">
-        <v>116.7398659</v>
+        <v>328726000</v>
       </c>
       <c r="AQ3" t="n">
-        <v>120.8643507</v>
+        <v>328726000</v>
       </c>
       <c r="AR3" t="n">
-        <v>125.1299356</v>
+        <v>328726000</v>
       </c>
       <c r="AS3" t="n">
-        <v>129.5412485</v>
+        <v>328726000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>General</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>va_industrial_mmm_usd</t>
+          <t>climate_change_factor_gnrl_hydropower_availability</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -870,126 +873,126 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J4" t="n">
-        <v>10.64896106</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>10.93995588</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>11.22497854</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>11.80920172</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>12.14492665</v>
+        <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>12.47977591</v>
+        <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>12.84997243</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>13.2460467</v>
+        <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>13.68496934</v>
+        <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>14.16767585</v>
+        <v>1</v>
       </c>
       <c r="T4" t="n">
-        <v>14.67048758</v>
+        <v>1</v>
       </c>
       <c r="U4" t="n">
-        <v>15.19425785</v>
+        <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>15.73988515</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
-        <v>16.30831534</v>
+        <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>16.9005455</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
-        <v>17.51762663</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="n">
-        <v>18.16066381</v>
+        <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>18.83081376</v>
+        <v>1</v>
       </c>
       <c r="AB4" t="n">
-        <v>19.52929278</v>
+        <v>1</v>
       </c>
       <c r="AC4" t="n">
-        <v>20.25736572</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="n">
-        <v>21.01636007</v>
+        <v>1</v>
       </c>
       <c r="AE4" t="n">
-        <v>21.80766246</v>
+        <v>1</v>
       </c>
       <c r="AF4" t="n">
-        <v>22.63271908</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="n">
-        <v>23.49303873</v>
+        <v>1</v>
       </c>
       <c r="AH4" t="n">
-        <v>24.39018952</v>
+        <v>1</v>
       </c>
       <c r="AI4" t="n">
-        <v>25.32580491</v>
+        <v>1</v>
       </c>
       <c r="AJ4" t="n">
-        <v>26.3015873</v>
+        <v>1</v>
       </c>
       <c r="AK4" t="n">
-        <v>27.31930573</v>
+        <v>1</v>
       </c>
       <c r="AL4" t="n">
-        <v>28.38080567</v>
+        <v>1</v>
       </c>
       <c r="AM4" t="n">
-        <v>29.48801404</v>
+        <v>1</v>
       </c>
       <c r="AN4" t="n">
-        <v>30.64292727</v>
+        <v>1</v>
       </c>
       <c r="AO4" t="n">
-        <v>31.84761623</v>
+        <v>1</v>
       </c>
       <c r="AP4" t="n">
-        <v>33.10423441</v>
+        <v>1</v>
       </c>
       <c r="AQ4" t="n">
-        <v>34.41501926</v>
+        <v>1</v>
       </c>
       <c r="AR4" t="n">
-        <v>35.78229664</v>
+        <v>1</v>
       </c>
       <c r="AS4" t="n">
-        <v>37.20848398</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>General</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>va_manufacturing_mmm_usd</t>
+          <t>elasticity_gnrl_rate_occupancy_to_gdppc</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1004,123 +1007,123 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>6.239061372</v>
+        <v>-0.1</v>
       </c>
       <c r="K5" t="n">
-        <v>6.518427514</v>
+        <v>-0.1</v>
       </c>
       <c r="L5" t="n">
-        <v>6.936925587999999</v>
+        <v>-0.1</v>
       </c>
       <c r="M5" t="n">
-        <v>7.196583448999999</v>
+        <v>-0.1</v>
       </c>
       <c r="N5" t="n">
-        <v>7.402811149</v>
+        <v>-0.1</v>
       </c>
       <c r="O5" t="n">
-        <v>7.607812281</v>
+        <v>-0.1</v>
       </c>
       <c r="P5" t="n">
-        <v>7.833481796</v>
+        <v>-0.1</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.074160761</v>
+        <v>-0.1</v>
       </c>
       <c r="R5" t="n">
-        <v>8.340166596</v>
+        <v>-0.1</v>
       </c>
       <c r="S5" t="n">
-        <v>8.632126082999999</v>
+        <v>-0.1</v>
       </c>
       <c r="T5" t="n">
-        <v>8.935810937999999</v>
+        <v>-0.1</v>
       </c>
       <c r="U5" t="n">
-        <v>9.251868677999999</v>
+        <v>-0.1</v>
       </c>
       <c r="V5" t="n">
-        <v>9.580973605000001</v>
+        <v>-0.1</v>
       </c>
       <c r="W5" t="n">
-        <v>9.923833127</v>
+        <v>-0.1</v>
       </c>
       <c r="X5" t="n">
-        <v>10.28118606</v>
+        <v>-0.1</v>
       </c>
       <c r="Y5" t="n">
-        <v>10.65380161</v>
+        <v>-0.1</v>
       </c>
       <c r="Z5" t="n">
-        <v>11.04248122</v>
+        <v>-0.1</v>
       </c>
       <c r="AA5" t="n">
-        <v>11.44806257</v>
+        <v>-0.1</v>
       </c>
       <c r="AB5" t="n">
-        <v>11.87141183</v>
+        <v>-0.1</v>
       </c>
       <c r="AC5" t="n">
-        <v>12.31343688</v>
+        <v>-0.1</v>
       </c>
       <c r="AD5" t="n">
-        <v>12.77507543</v>
+        <v>-0.1</v>
       </c>
       <c r="AE5" t="n">
-        <v>13.25730139</v>
+        <v>-0.1</v>
       </c>
       <c r="AF5" t="n">
-        <v>13.76112757</v>
+        <v>-0.1</v>
       </c>
       <c r="AG5" t="n">
-        <v>14.28760694</v>
+        <v>-0.1</v>
       </c>
       <c r="AH5" t="n">
-        <v>14.83783832</v>
+        <v>-0.1</v>
       </c>
       <c r="AI5" t="n">
-        <v>15.41296606</v>
+        <v>-0.1</v>
       </c>
       <c r="AJ5" t="n">
-        <v>16.01418179</v>
+        <v>-0.1</v>
       </c>
       <c r="AK5" t="n">
-        <v>16.64272962</v>
+        <v>-0.1</v>
       </c>
       <c r="AL5" t="n">
-        <v>17.29990504</v>
+        <v>-0.1</v>
       </c>
       <c r="AM5" t="n">
-        <v>17.98705684</v>
+        <v>-0.1</v>
       </c>
       <c r="AN5" t="n">
-        <v>18.7055965</v>
+        <v>-0.1</v>
       </c>
       <c r="AO5" t="n">
-        <v>19.45699951</v>
+        <v>-0.1</v>
       </c>
       <c r="AP5" t="n">
-        <v>20.24280569</v>
+        <v>-0.1</v>
       </c>
       <c r="AQ5" t="n">
-        <v>21.0646224</v>
+        <v>-0.1</v>
       </c>
       <c r="AR5" t="n">
-        <v>21.92412658</v>
+        <v>-0.1</v>
       </c>
       <c r="AS5" t="n">
-        <v>22.82306754</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>General</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>va_mining_mmm_usd</t>
+          <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1135,112 +1138,112 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>2.954671495</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>3.080126548</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>3.183768001</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>3.266669999</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>3.361588594</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>3.455923617</v>
+        <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>3.560140589</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.67142209</v>
+        <v>1</v>
       </c>
       <c r="R6" t="n">
-        <v>3.794604334</v>
+        <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>3.929847167</v>
+        <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>4.07019666</v>
+        <v>1</v>
       </c>
       <c r="U6" t="n">
-        <v>4.215823087</v>
+        <v>1</v>
       </c>
       <c r="V6" t="n">
-        <v>4.366906548</v>
+        <v>1</v>
       </c>
       <c r="W6" t="n">
-        <v>4.5236353</v>
+        <v>1</v>
       </c>
       <c r="X6" t="n">
-        <v>4.686207257</v>
+        <v>1</v>
       </c>
       <c r="Y6" t="n">
-        <v>4.854831048</v>
+        <v>1</v>
       </c>
       <c r="Z6" t="n">
-        <v>5.029725587</v>
+        <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>5.211118257</v>
+        <v>1</v>
       </c>
       <c r="AB6" t="n">
-        <v>5.399249713</v>
+        <v>1</v>
       </c>
       <c r="AC6" t="n">
-        <v>5.594366965</v>
+        <v>1</v>
       </c>
       <c r="AD6" t="n">
-        <v>5.796731138999999</v>
+        <v>1</v>
       </c>
       <c r="AE6" t="n">
-        <v>6.006614932000001</v>
+        <v>1</v>
       </c>
       <c r="AF6" t="n">
-        <v>6.224302253999999</v>
+        <v>1</v>
       </c>
       <c r="AG6" t="n">
-        <v>6.450089021</v>
+        <v>1</v>
       </c>
       <c r="AH6" t="n">
-        <v>6.68428089</v>
+        <v>1</v>
       </c>
       <c r="AI6" t="n">
-        <v>6.927195331</v>
+        <v>1</v>
       </c>
       <c r="AJ6" t="n">
-        <v>7.179162458</v>
+        <v>1</v>
       </c>
       <c r="AK6" t="n">
-        <v>7.440523291</v>
+        <v>1</v>
       </c>
       <c r="AL6" t="n">
-        <v>7.711633128</v>
+        <v>1</v>
       </c>
       <c r="AM6" t="n">
-        <v>7.992862845</v>
+        <v>1</v>
       </c>
       <c r="AN6" t="n">
-        <v>8.284593465</v>
+        <v>1</v>
       </c>
       <c r="AO6" t="n">
-        <v>8.587217436</v>
+        <v>1</v>
       </c>
       <c r="AP6" t="n">
-        <v>8.901141124</v>
+        <v>1</v>
       </c>
       <c r="AQ6" t="n">
-        <v>9.226784771</v>
+        <v>1</v>
       </c>
       <c r="AR6" t="n">
-        <v>9.564583555</v>
+        <v>1</v>
       </c>
       <c r="AS6" t="n">
-        <v>9.914988205</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1251,7 +1254,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>area_gnrl_country_ha</t>
+          <t>limit_gnrl_annual_emissions_mt_ch4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -1266,112 +1269,112 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="K7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="L7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="M7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="N7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="O7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="P7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="Q7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="R7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="S7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="T7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="U7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="V7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="W7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="X7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="Y7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="Z7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AA7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AB7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AC7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AD7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AE7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AF7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AG7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AH7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AI7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AJ7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AK7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AL7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AM7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AN7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AO7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AP7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AQ7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AR7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
       <c r="AS7" t="n">
-        <v>328726000</v>
+        <v>-999</v>
       </c>
     </row>
     <row r="8">
@@ -1382,7 +1385,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>elasticity_gnrl_rate_occupancy_to_gdppc</t>
+          <t>limit_gnrl_annual_emissions_mt_co2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1397,112 +1400,112 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AE8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AF8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AG8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AH8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AI8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AJ8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AK8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AL8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AM8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AN8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AO8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AP8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AQ8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AR8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
       <c r="AS8" t="n">
-        <v>-0.1</v>
+        <v>-999</v>
       </c>
     </row>
     <row r="9">
@@ -1513,7 +1516,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>frac_gnrl_eating_red_meat</t>
+          <t>limit_gnrl_annual_emissions_mt_n2o</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1528,112 +1531,112 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="K9" t="n">
-        <v>0.99</v>
+        <v>-999</v>
       </c>
       <c r="L9" t="n">
-        <v>0.98</v>
+        <v>-999</v>
       </c>
       <c r="M9" t="n">
-        <v>0.97</v>
+        <v>-999</v>
       </c>
       <c r="N9" t="n">
-        <v>0.96</v>
+        <v>-999</v>
       </c>
       <c r="O9" t="n">
-        <v>0.95</v>
+        <v>-999</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9399999999999999</v>
+        <v>-999</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.93</v>
+        <v>-999</v>
       </c>
       <c r="R9" t="n">
-        <v>0.92</v>
+        <v>-999</v>
       </c>
       <c r="S9" t="n">
-        <v>0.91</v>
+        <v>-999</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="U9" t="n">
-        <v>0.89</v>
+        <v>-999</v>
       </c>
       <c r="V9" t="n">
-        <v>0.88</v>
+        <v>-999</v>
       </c>
       <c r="W9" t="n">
-        <v>0.87</v>
+        <v>-999</v>
       </c>
       <c r="X9" t="n">
-        <v>0.86</v>
+        <v>-999</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.85</v>
+        <v>-999</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.84</v>
+        <v>-999</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.83</v>
+        <v>-999</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.82</v>
+        <v>-999</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.8100000000000001</v>
+        <v>-999</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.8</v>
+        <v>-999</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.79</v>
+        <v>-999</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.78</v>
+        <v>-999</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.77</v>
+        <v>-999</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.76</v>
+        <v>-999</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.75</v>
+        <v>-999</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.74</v>
+        <v>-999</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.73</v>
+        <v>-999</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.72</v>
+        <v>-999</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.71</v>
+        <v>-999</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.7</v>
+        <v>-999</v>
       </c>
     </row>
     <row r="10">
@@ -1644,7 +1647,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>limit_gnrl_annual_emissions_mt_ch4</t>
+          <t>occrateinit_gnrl_occupancy</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1659,112 +1662,112 @@
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="K10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="L10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="M10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="N10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="O10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="P10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="Q10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="R10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="S10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="T10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="U10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="V10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="W10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="X10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="Y10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="Z10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AA10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AB10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AC10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AD10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AE10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AF10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AG10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AH10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AI10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AK10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AL10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AM10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AN10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AO10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AP10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AQ10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AR10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
       <c r="AS10" t="n">
-        <v>-999</v>
+        <v>4.698333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -1775,7 +1778,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>limit_gnrl_annual_emissions_mt_co2</t>
+          <t>population_gnrl_rural</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1790,112 +1793,112 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>-999</v>
+        <v>880723742.47416</v>
       </c>
       <c r="K11" t="n">
-        <v>-999</v>
+        <v>885015936.105</v>
       </c>
       <c r="L11" t="n">
-        <v>-999</v>
+        <v>888881381.256</v>
       </c>
       <c r="M11" t="n">
-        <v>-999</v>
+        <v>892338114.0951</v>
       </c>
       <c r="N11" t="n">
-        <v>-999</v>
+        <v>895386227.15168</v>
       </c>
       <c r="O11" t="n">
-        <v>-999</v>
+        <v>898024053.4949</v>
       </c>
       <c r="P11" t="n">
-        <v>-999</v>
+        <v>906856770.098022</v>
       </c>
       <c r="Q11" t="n">
-        <v>-999</v>
+        <v>910428206.9478641</v>
       </c>
       <c r="R11" t="n">
-        <v>-999</v>
+        <v>913999643.797706</v>
       </c>
       <c r="S11" t="n">
-        <v>-999</v>
+        <v>917571080.647548</v>
       </c>
       <c r="T11" t="n">
-        <v>-999</v>
+        <v>921142517.49739</v>
       </c>
       <c r="U11" t="n">
-        <v>-999</v>
+        <v>923271168.479228</v>
       </c>
       <c r="V11" t="n">
-        <v>-999</v>
+        <v>925399819.461066</v>
       </c>
       <c r="W11" t="n">
-        <v>-999</v>
+        <v>927528470.442904</v>
       </c>
       <c r="X11" t="n">
-        <v>-999</v>
+        <v>929657121.424742</v>
       </c>
       <c r="Y11" t="n">
-        <v>-999</v>
+        <v>931785772.40658</v>
       </c>
       <c r="Z11" t="n">
-        <v>-999</v>
+        <v>932777441.008715</v>
       </c>
       <c r="AA11" t="n">
-        <v>-999</v>
+        <v>933769109.61085</v>
       </c>
       <c r="AB11" t="n">
-        <v>-999</v>
+        <v>934760778.2129848</v>
       </c>
       <c r="AC11" t="n">
-        <v>-999</v>
+        <v>935752446.81512</v>
       </c>
       <c r="AD11" t="n">
-        <v>-999</v>
+        <v>936744115.417255</v>
       </c>
       <c r="AE11" t="n">
-        <v>-999</v>
+        <v>936499448.546204</v>
       </c>
       <c r="AF11" t="n">
-        <v>-999</v>
+        <v>936254781.6751528</v>
       </c>
       <c r="AG11" t="n">
-        <v>-999</v>
+        <v>936010114.8041019</v>
       </c>
       <c r="AH11" t="n">
-        <v>-999</v>
+        <v>935765447.933051</v>
       </c>
       <c r="AI11" t="n">
-        <v>-999</v>
+        <v>935520781.062</v>
       </c>
       <c r="AJ11" t="n">
-        <v>-999</v>
+        <v>934079056.656969</v>
       </c>
       <c r="AK11" t="n">
-        <v>-999</v>
+        <v>932637332.251938</v>
       </c>
       <c r="AL11" t="n">
-        <v>-999</v>
+        <v>931195607.846907</v>
       </c>
       <c r="AM11" t="n">
-        <v>-999</v>
+        <v>929753883.4418761</v>
       </c>
       <c r="AN11" t="n">
-        <v>-999</v>
+        <v>928312159.036845</v>
       </c>
       <c r="AO11" t="n">
-        <v>-999</v>
+        <v>925471525.202664</v>
       </c>
       <c r="AP11" t="n">
-        <v>-999</v>
+        <v>922630891.3684832</v>
       </c>
       <c r="AQ11" t="n">
-        <v>-999</v>
+        <v>919790257.534302</v>
       </c>
       <c r="AR11" t="n">
-        <v>-999</v>
+        <v>916949623.700121</v>
       </c>
       <c r="AS11" t="n">
-        <v>-999</v>
+        <v>914108989.86594</v>
       </c>
     </row>
     <row r="12">
@@ -1906,7 +1909,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>limit_gnrl_annual_emissions_mt_n2o</t>
+          <t>population_gnrl_urban</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1921,505 +1924,1027 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-999</v>
+        <v>429428649.52584</v>
       </c>
       <c r="K12" t="n">
-        <v>-999</v>
+        <v>439501313.895</v>
       </c>
       <c r="L12" t="n">
-        <v>-999</v>
+        <v>449795397.744</v>
       </c>
       <c r="M12" t="n">
-        <v>-999</v>
+        <v>460304168.9049</v>
       </c>
       <c r="N12" t="n">
-        <v>-999</v>
+        <v>471031528.84832</v>
       </c>
       <c r="O12" t="n">
-        <v>-999</v>
+        <v>481980331.5051</v>
       </c>
       <c r="P12" t="n">
-        <v>-999</v>
+        <v>495969063.101978</v>
       </c>
       <c r="Q12" t="n">
-        <v>-999</v>
+        <v>507134002.452136</v>
       </c>
       <c r="R12" t="n">
-        <v>-999</v>
+        <v>518298941.802294</v>
       </c>
       <c r="S12" t="n">
-        <v>-999</v>
+        <v>529463881.1524519</v>
       </c>
       <c r="T12" t="n">
-        <v>-999</v>
+        <v>540628820.50261</v>
       </c>
       <c r="U12" t="n">
-        <v>-999</v>
+        <v>551864940.720772</v>
       </c>
       <c r="V12" t="n">
-        <v>-999</v>
+        <v>563101060.938934</v>
       </c>
       <c r="W12" t="n">
-        <v>-999</v>
+        <v>574337181.157096</v>
       </c>
       <c r="X12" t="n">
-        <v>-999</v>
+        <v>585573301.375258</v>
       </c>
       <c r="Y12" t="n">
-        <v>-999</v>
+        <v>596809421.59342</v>
       </c>
       <c r="Z12" t="n">
-        <v>-999</v>
+        <v>608186310.7912849</v>
       </c>
       <c r="AA12" t="n">
-        <v>-999</v>
+        <v>619563199.98915</v>
       </c>
       <c r="AB12" t="n">
-        <v>-999</v>
+        <v>630940089.1870151</v>
       </c>
       <c r="AC12" t="n">
-        <v>-999</v>
+        <v>642316978.3848799</v>
       </c>
       <c r="AD12" t="n">
-        <v>-999</v>
+        <v>653693867.5827451</v>
       </c>
       <c r="AE12" t="n">
-        <v>-999</v>
+        <v>665027848.853796</v>
       </c>
       <c r="AF12" t="n">
-        <v>-999</v>
+        <v>676361830.1248469</v>
       </c>
       <c r="AG12" t="n">
-        <v>-999</v>
+        <v>687695811.3958981</v>
       </c>
       <c r="AH12" t="n">
-        <v>-999</v>
+        <v>699029792.666949</v>
       </c>
       <c r="AI12" t="n">
-        <v>-999</v>
+        <v>710363773.9380001</v>
       </c>
       <c r="AJ12" t="n">
-        <v>-999</v>
+        <v>721543059.943031</v>
       </c>
       <c r="AK12" t="n">
-        <v>-999</v>
+        <v>732722345.9480621</v>
       </c>
       <c r="AL12" t="n">
-        <v>-999</v>
+        <v>743901631.9530929</v>
       </c>
       <c r="AM12" t="n">
-        <v>-999</v>
+        <v>755080917.958124</v>
       </c>
       <c r="AN12" t="n">
-        <v>-999</v>
+        <v>766260203.963155</v>
       </c>
       <c r="AO12" t="n">
-        <v>-999</v>
+        <v>776945460.797336</v>
       </c>
       <c r="AP12" t="n">
-        <v>-999</v>
+        <v>787630717.6315169</v>
       </c>
       <c r="AQ12" t="n">
-        <v>-999</v>
+        <v>798315974.465698</v>
       </c>
       <c r="AR12" t="n">
-        <v>-999</v>
+        <v>809001231.299879</v>
       </c>
       <c r="AS12" t="n">
-        <v>-999</v>
+        <v>819686488.1340599</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>occrateinit_gnrl_occupancy</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="K13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="M13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="N13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="O13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="P13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="R13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="S13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="T13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="U13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="V13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="W13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="X13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AI13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AK13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AL13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AM13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AR13" t="n">
-        <v>4.69833333333333</v>
-      </c>
-      <c r="AS13" t="n">
-        <v>4.69833333333333</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9600000000000001</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>population_gnrl_rural</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" t="n">
-        <v>880723742.47416</v>
-      </c>
-      <c r="K14" t="n">
-        <v>885015936.105</v>
-      </c>
-      <c r="L14" t="n">
-        <v>888881381.256</v>
-      </c>
-      <c r="M14" t="n">
-        <v>892338114.0951</v>
-      </c>
-      <c r="N14" t="n">
-        <v>895386227.15168</v>
-      </c>
-      <c r="O14" t="n">
-        <v>898024053.4949</v>
-      </c>
-      <c r="P14" t="n">
-        <v>906856770.098022</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>910428206.9478641</v>
-      </c>
-      <c r="R14" t="n">
-        <v>913999643.797706</v>
-      </c>
-      <c r="S14" t="n">
-        <v>917571080.647548</v>
-      </c>
-      <c r="T14" t="n">
-        <v>921142517.49739</v>
-      </c>
-      <c r="U14" t="n">
-        <v>923271168.479228</v>
-      </c>
-      <c r="V14" t="n">
-        <v>925399819.461066</v>
-      </c>
-      <c r="W14" t="n">
-        <v>927528470.442904</v>
-      </c>
-      <c r="X14" t="n">
-        <v>929657121.424742</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>931785772.40658</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>932777441.008715</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>933769109.61085</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>934760778.212985</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>935752446.81512</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>936744115.417255</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>936499448.546204</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>936254781.675153</v>
-      </c>
-      <c r="AG14" t="n">
-        <v>936010114.8041019</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>935765447.933051</v>
-      </c>
-      <c r="AI14" t="n">
-        <v>935520781.062</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>934079056.656969</v>
-      </c>
-      <c r="AK14" t="n">
-        <v>932637332.251938</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>931195607.846907</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>929753883.4418761</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>928312159.036845</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>925471525.202664</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>922630891.3684829</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>919790257.534302</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>916949623.700121</v>
-      </c>
-      <c r="AS14" t="n">
-        <v>914108989.86594</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9600000000000001</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>General</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>population_gnrl_urban</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" t="n">
-        <v>429428649.52584</v>
-      </c>
-      <c r="K15" t="n">
-        <v>439501313.895</v>
-      </c>
-      <c r="L15" t="n">
-        <v>449795397.744</v>
-      </c>
-      <c r="M15" t="n">
-        <v>460304168.9049</v>
-      </c>
-      <c r="N15" t="n">
-        <v>471031528.84832</v>
-      </c>
-      <c r="O15" t="n">
-        <v>481980331.5051</v>
-      </c>
-      <c r="P15" t="n">
-        <v>495969063.101978</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>507134002.452136</v>
-      </c>
-      <c r="R15" t="n">
-        <v>518298941.802294</v>
-      </c>
-      <c r="S15" t="n">
-        <v>529463881.152452</v>
-      </c>
-      <c r="T15" t="n">
-        <v>540628820.50261</v>
-      </c>
-      <c r="U15" t="n">
-        <v>551864940.720772</v>
-      </c>
-      <c r="V15" t="n">
-        <v>563101060.938934</v>
-      </c>
-      <c r="W15" t="n">
-        <v>574337181.157096</v>
-      </c>
-      <c r="X15" t="n">
-        <v>585573301.375258</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>596809421.59342</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>608186310.791285</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>619563199.98915</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>630940089.1870151</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>642316978.3848799</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>653693867.582745</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>665027848.853796</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>676361830.1248471</v>
-      </c>
-      <c r="AG15" t="n">
-        <v>687695811.395898</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>699029792.666949</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>710363773.938</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>721543059.943031</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>732722345.9480619</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>743901631.9530931</v>
-      </c>
-      <c r="AM15" t="n">
-        <v>755080917.958124</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>766260203.963155</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>776945460.797336</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>787630717.6315171</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>798315974.465698</v>
-      </c>
-      <c r="AR15" t="n">
-        <v>809001231.299879</v>
-      </c>
-      <c r="AS15" t="n">
-        <v>819686488.13406</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9600000000000001</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update, added model_variable. Final before branching to start work on new ModelAttributes system.
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:BM12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,24 +449,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>variable_trajectory_group_trajectory_type</t>
@@ -474,12 +474,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>max_35</t>
+          <t>max_55</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>min_35</t>
+          <t>min_55</t>
         </is>
       </c>
       <c r="J1" s="1" t="n">
@@ -589,6 +589,66 @@
       </c>
       <c r="AS1" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -620,34 +680,34 @@
         <v>5978.1806666</v>
       </c>
       <c r="L2" t="n">
-        <v>6257.3136702</v>
+        <v>6257.313670200001</v>
       </c>
       <c r="M2" t="n">
-        <v>6536.4466738</v>
+        <v>6536.446673800001</v>
       </c>
       <c r="N2" t="n">
-        <v>6815.5796774</v>
+        <v>6815.579677400001</v>
       </c>
       <c r="O2" t="n">
-        <v>7094.712681</v>
+        <v>7094.712681000001</v>
       </c>
       <c r="P2" t="n">
-        <v>7571.8407134</v>
+        <v>7571.840713400001</v>
       </c>
       <c r="Q2" t="n">
-        <v>8048.9687458</v>
+        <v>8048.968745800003</v>
       </c>
       <c r="R2" t="n">
-        <v>8526.096778200001</v>
+        <v>8526.096778200004</v>
       </c>
       <c r="S2" t="n">
-        <v>9003.224810600001</v>
+        <v>9003.224810600004</v>
       </c>
       <c r="T2" t="n">
-        <v>9480.352843000001</v>
+        <v>9480.352843000004</v>
       </c>
       <c r="U2" t="n">
-        <v>9999.1814144</v>
+        <v>9999.181414400004</v>
       </c>
       <c r="V2" t="n">
         <v>10518.0099858</v>
@@ -680,46 +740,106 @@
         <v>15720.860502</v>
       </c>
       <c r="AF2" t="n">
-        <v>16402.394764</v>
+        <v>16402.39476400002</v>
       </c>
       <c r="AG2" t="n">
-        <v>17083.929026</v>
+        <v>17083.92902600002</v>
       </c>
       <c r="AH2" t="n">
-        <v>17765.463288</v>
+        <v>17765.46328800002</v>
       </c>
       <c r="AI2" t="n">
-        <v>18446.99755</v>
+        <v>18446.99755000002</v>
       </c>
       <c r="AJ2" t="n">
-        <v>19206.924266</v>
+        <v>19206.92426600002</v>
       </c>
       <c r="AK2" t="n">
-        <v>19966.850982</v>
+        <v>19966.85098200002</v>
       </c>
       <c r="AL2" t="n">
-        <v>20726.777698</v>
+        <v>20726.77769800002</v>
       </c>
       <c r="AM2" t="n">
-        <v>21486.704414</v>
+        <v>21486.70441400002</v>
       </c>
       <c r="AN2" t="n">
-        <v>22246.63113</v>
+        <v>22246.63113000002</v>
       </c>
       <c r="AO2" t="n">
-        <v>23076.367234</v>
+        <v>23076.36723400002</v>
       </c>
       <c r="AP2" t="n">
-        <v>23906.103338</v>
+        <v>23906.10333800003</v>
       </c>
       <c r="AQ2" t="n">
-        <v>24735.839442</v>
+        <v>24735.83944200003</v>
       </c>
       <c r="AR2" t="n">
-        <v>25565.575546</v>
+        <v>25565.57554600003</v>
       </c>
       <c r="AS2" t="n">
-        <v>26395.31165</v>
+        <v>26395.31165000003</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>27273.40450150054</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>28162.23718332734</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>29060.93273098747</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>29968.56370866613</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>30884.15306034566</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>31806.67516575942</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>32735.05710360175</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>33668.18012351037</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>34604.88132738751</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>35543.95555963519</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>36484.15750485686</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>37424.20399052605</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>38362.77649104803</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>39298.52382855237</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>40230.06506465726</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>41155.99257634703</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>42074.8753080102</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>42985.26219060671</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>43885.68571787133</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>44774.66566842715</v>
       </c>
     </row>
     <row r="3">
@@ -852,6 +972,66 @@
       <c r="AS3" t="n">
         <v>328726000</v>
       </c>
+      <c r="AT3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>328726000</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>328726000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -983,6 +1163,66 @@
       <c r="AS4" t="n">
         <v>1</v>
       </c>
+      <c r="AT4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1114,6 +1354,66 @@
       <c r="AS5" t="n">
         <v>-0.1</v>
       </c>
+      <c r="AT5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>-0.1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1126,7 +1426,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -1138,112 +1440,172 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Q6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="U6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="V6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="W6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="X6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AA6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AB6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AC6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AD6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AE6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AF6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AG6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AH6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AI6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AK6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AL6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AM6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AN6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AO6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AP6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AR6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="AS6" t="n">
-        <v>1</v>
+        <v>0.31</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.31</v>
       </c>
     </row>
     <row r="7">
@@ -1376,6 +1738,66 @@
       <c r="AS7" t="n">
         <v>-999</v>
       </c>
+      <c r="AT7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>-999</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1507,6 +1929,66 @@
       <c r="AS8" t="n">
         <v>-999</v>
       </c>
+      <c r="AT8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>-999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1638,6 +2120,66 @@
       <c r="AS9" t="n">
         <v>-999</v>
       </c>
+      <c r="AT9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>-999</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>-999</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1769,6 +2311,66 @@
       <c r="AS10" t="n">
         <v>4.698333333333333</v>
       </c>
+      <c r="AT10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>4.698333333333333</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>4.698333333333333</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1799,106 +2401,166 @@
         <v>885015936.105</v>
       </c>
       <c r="L11" t="n">
-        <v>888881381.256</v>
+        <v>888881381.2559999</v>
       </c>
       <c r="M11" t="n">
-        <v>892338114.0951</v>
+        <v>892338114.0951002</v>
       </c>
       <c r="N11" t="n">
-        <v>895386227.15168</v>
+        <v>895386227.1516801</v>
       </c>
       <c r="O11" t="n">
-        <v>898024053.4949</v>
+        <v>898024053.4949002</v>
       </c>
       <c r="P11" t="n">
-        <v>906856770.098022</v>
+        <v>906856770.0980221</v>
       </c>
       <c r="Q11" t="n">
-        <v>910428206.9478641</v>
+        <v>910428206.9478642</v>
       </c>
       <c r="R11" t="n">
-        <v>913999643.797706</v>
+        <v>913999643.7977062</v>
       </c>
       <c r="S11" t="n">
-        <v>917571080.647548</v>
+        <v>917571080.6475483</v>
       </c>
       <c r="T11" t="n">
-        <v>921142517.49739</v>
+        <v>921142517.4973904</v>
       </c>
       <c r="U11" t="n">
-        <v>923271168.479228</v>
+        <v>923271168.4792284</v>
       </c>
       <c r="V11" t="n">
-        <v>925399819.461066</v>
+        <v>925399819.4610667</v>
       </c>
       <c r="W11" t="n">
-        <v>927528470.442904</v>
+        <v>927528470.4429048</v>
       </c>
       <c r="X11" t="n">
-        <v>929657121.424742</v>
+        <v>929657121.4247428</v>
       </c>
       <c r="Y11" t="n">
-        <v>931785772.40658</v>
+        <v>931785772.4065808</v>
       </c>
       <c r="Z11" t="n">
-        <v>932777441.008715</v>
+        <v>932777441.0087162</v>
       </c>
       <c r="AA11" t="n">
-        <v>933769109.61085</v>
+        <v>933769109.6108512</v>
       </c>
       <c r="AB11" t="n">
-        <v>934760778.2129848</v>
+        <v>934760778.2129862</v>
       </c>
       <c r="AC11" t="n">
-        <v>935752446.81512</v>
+        <v>935752446.8151214</v>
       </c>
       <c r="AD11" t="n">
-        <v>936744115.417255</v>
+        <v>936744115.4172565</v>
       </c>
       <c r="AE11" t="n">
-        <v>936499448.546204</v>
+        <v>936499448.5462054</v>
       </c>
       <c r="AF11" t="n">
-        <v>936254781.6751528</v>
+        <v>936254781.6751541</v>
       </c>
       <c r="AG11" t="n">
-        <v>936010114.8041019</v>
+        <v>936010114.8041033</v>
       </c>
       <c r="AH11" t="n">
-        <v>935765447.933051</v>
+        <v>935765447.9330523</v>
       </c>
       <c r="AI11" t="n">
-        <v>935520781.062</v>
+        <v>935520781.0620012</v>
       </c>
       <c r="AJ11" t="n">
-        <v>934079056.656969</v>
+        <v>934079056.6569703</v>
       </c>
       <c r="AK11" t="n">
-        <v>932637332.251938</v>
+        <v>932637332.2519392</v>
       </c>
       <c r="AL11" t="n">
-        <v>931195607.846907</v>
+        <v>931195607.8469083</v>
       </c>
       <c r="AM11" t="n">
-        <v>929753883.4418761</v>
+        <v>929753883.4418772</v>
       </c>
       <c r="AN11" t="n">
-        <v>928312159.036845</v>
+        <v>928312159.0368462</v>
       </c>
       <c r="AO11" t="n">
-        <v>925471525.202664</v>
+        <v>925471525.2026653</v>
       </c>
       <c r="AP11" t="n">
-        <v>922630891.3684832</v>
+        <v>922630891.3684845</v>
       </c>
       <c r="AQ11" t="n">
-        <v>919790257.534302</v>
+        <v>919790257.5343034</v>
       </c>
       <c r="AR11" t="n">
-        <v>916949623.700121</v>
+        <v>916949623.7001225</v>
       </c>
       <c r="AS11" t="n">
-        <v>914108989.86594</v>
+        <v>914108989.8659414</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>910528891.5603858</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>906696344.2374226</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>902614158.694883</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>898285381.6000795</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>893713289.584669</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>888901383.1606724</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>883853380.4504673</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>878573210.7267025</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>873065007.7607515</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>867333102.9806495</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>861382018.4414332</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>855216459.6125952</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>848841307.9888465</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>842261613.5317464</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>835482586.9509113</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>828509591.834545</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>821348136.6399161</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>814003866.5551914</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>806482555.2447132</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>798790096.4903572</v>
       </c>
     </row>
     <row r="12">
@@ -1945,7 +2607,7 @@
         <v>495969063.101978</v>
       </c>
       <c r="Q12" t="n">
-        <v>507134002.452136</v>
+        <v>507134002.4521359</v>
       </c>
       <c r="R12" t="n">
         <v>518298941.802294</v>
@@ -1957,79 +2619,139 @@
         <v>540628820.50261</v>
       </c>
       <c r="U12" t="n">
-        <v>551864940.720772</v>
+        <v>551864940.7207718</v>
       </c>
       <c r="V12" t="n">
-        <v>563101060.938934</v>
+        <v>563101060.9389338</v>
       </c>
       <c r="W12" t="n">
-        <v>574337181.157096</v>
+        <v>574337181.1570959</v>
       </c>
       <c r="X12" t="n">
-        <v>585573301.375258</v>
+        <v>585573301.3752576</v>
       </c>
       <c r="Y12" t="n">
-        <v>596809421.59342</v>
+        <v>596809421.5934196</v>
       </c>
       <c r="Z12" t="n">
-        <v>608186310.7912849</v>
+        <v>608186310.7912844</v>
       </c>
       <c r="AA12" t="n">
-        <v>619563199.98915</v>
+        <v>619563199.9891495</v>
       </c>
       <c r="AB12" t="n">
-        <v>630940089.1870151</v>
+        <v>630940089.1870143</v>
       </c>
       <c r="AC12" t="n">
-        <v>642316978.3848799</v>
+        <v>642316978.3848792</v>
       </c>
       <c r="AD12" t="n">
-        <v>653693867.5827451</v>
+        <v>653693867.5827446</v>
       </c>
       <c r="AE12" t="n">
-        <v>665027848.853796</v>
+        <v>665027848.8537955</v>
       </c>
       <c r="AF12" t="n">
-        <v>676361830.1248469</v>
+        <v>676361830.1248465</v>
       </c>
       <c r="AG12" t="n">
-        <v>687695811.3958981</v>
+        <v>687695811.3958975</v>
       </c>
       <c r="AH12" t="n">
-        <v>699029792.666949</v>
+        <v>699029792.6669484</v>
       </c>
       <c r="AI12" t="n">
-        <v>710363773.9380001</v>
+        <v>710363773.9379994</v>
       </c>
       <c r="AJ12" t="n">
-        <v>721543059.943031</v>
+        <v>721543059.9430304</v>
       </c>
       <c r="AK12" t="n">
-        <v>732722345.9480621</v>
+        <v>732722345.9480615</v>
       </c>
       <c r="AL12" t="n">
-        <v>743901631.9530929</v>
+        <v>743901631.9530923</v>
       </c>
       <c r="AM12" t="n">
-        <v>755080917.958124</v>
+        <v>755080917.9581234</v>
       </c>
       <c r="AN12" t="n">
-        <v>766260203.963155</v>
+        <v>766260203.9631542</v>
       </c>
       <c r="AO12" t="n">
-        <v>776945460.797336</v>
+        <v>776945460.7973353</v>
       </c>
       <c r="AP12" t="n">
-        <v>787630717.6315169</v>
+        <v>787630717.6315161</v>
       </c>
       <c r="AQ12" t="n">
-        <v>798315974.465698</v>
+        <v>798315974.4656971</v>
       </c>
       <c r="AR12" t="n">
-        <v>809001231.299879</v>
+        <v>809001231.2998779</v>
       </c>
       <c r="AS12" t="n">
-        <v>819686488.1340599</v>
+        <v>819686488.134059</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>829543972.0022355</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>839197415.0471984</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>848636337.648142</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>857850394.4485067</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>866829391.9584272</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>875563306.1631435</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>884042300.0841366</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>892256741.2407371</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>900197218.9608759</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>907854561.4905095</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>915219852.8521475</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>922284449.403839</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>929039996.0509217</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>935478442.0638708</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>941592056.456735</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>947373442.8818125</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>952815553.99755</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>957911705.2680538</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>962655588.1541128</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>967041282.6572597</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:BM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2064,24 +2786,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>variable_trajectory_group_trajectory_type</t>
@@ -2089,12 +2811,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>max_35</t>
+          <t>max_55</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>min_35</t>
+          <t>min_55</t>
         </is>
       </c>
       <c r="J1" s="1" t="n">
@@ -2204,6 +2926,66 @@
       </c>
       <c r="AS1" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -2217,7 +2999,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2229,112 +3013,172 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="U2" t="n">
-        <v>0.98</v>
+        <v>0.31</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9199999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.9</v>
+        <v>0.31</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.88</v>
+        <v>0.31</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.86</v>
+        <v>0.31</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.84</v>
+        <v>0.31</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8200000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.8</v>
+        <v>0.31</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.78</v>
+        <v>0.31</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.76</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.74</v>
+        <v>0.31</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.72</v>
+        <v>0.31</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.7</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.64</v>
+        <v>0.31</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.62</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.6</v>
+        <v>0.31</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.5800000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.54</v>
+        <v>0.31</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.52</v>
+        <v>0.31</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.5</v>
+        <v>0.31</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>
@@ -2348,7 +3192,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:BM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2369,24 +3213,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>variable_trajectory_group_trajectory_type</t>
@@ -2394,12 +3238,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>max_35</t>
+          <t>max_55</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>min_35</t>
+          <t>min_55</t>
         </is>
       </c>
       <c r="J1" s="1" t="n">
@@ -2509,6 +3353,66 @@
       </c>
       <c r="AS1" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -2522,7 +3426,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2534,112 +3440,172 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="U2" t="n">
-        <v>0.98</v>
+        <v>0.31</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9199999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.9</v>
+        <v>0.31</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.88</v>
+        <v>0.31</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.86</v>
+        <v>0.31</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.84</v>
+        <v>0.31</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8200000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.8</v>
+        <v>0.31</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.78</v>
+        <v>0.31</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.76</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.74</v>
+        <v>0.31</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.72</v>
+        <v>0.31</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.7</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.64</v>
+        <v>0.31</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.62</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.6</v>
+        <v>0.31</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.5800000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.54</v>
+        <v>0.31</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.52</v>
+        <v>0.31</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.5</v>
+        <v>0.31</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>
@@ -2653,7 +3619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:BM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2674,24 +3640,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>variable_trajectory_group_trajectory_type</t>
@@ -2699,12 +3665,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>max_35</t>
+          <t>max_55</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>min_35</t>
+          <t>min_55</t>
         </is>
       </c>
       <c r="J1" s="1" t="n">
@@ -2814,6 +3780,66 @@
       </c>
       <c r="AS1" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="2">
@@ -2827,7 +3853,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2839,112 +3867,172 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
       <c r="U2" t="n">
-        <v>0.98</v>
+        <v>0.31</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9199999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.9</v>
+        <v>0.31</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.88</v>
+        <v>0.31</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.86</v>
+        <v>0.31</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.84</v>
+        <v>0.31</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.8200000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.8</v>
+        <v>0.31</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.78</v>
+        <v>0.31</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.76</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.74</v>
+        <v>0.31</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.72</v>
+        <v>0.31</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.7</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.31</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.64</v>
+        <v>0.31</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.62</v>
+        <v>0.3099999999999999</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.6</v>
+        <v>0.31</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.5800000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.54</v>
+        <v>0.31</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.52</v>
+        <v>0.31</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.5</v>
+        <v>0.31</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a land use FAO crosswalk
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5004" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5007" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5009" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-6004" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4038,4 +4039,431 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BM2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_55</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_55</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.3100000000000001</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.3100000000000001</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.3099999999999999</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.3099999999999999</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed some minor issues with categories in IPCC LVST crosswalk
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/india/model_input_variables_india_se_calibrated.xlsx
@@ -798,7 +798,7 @@
         <v>30884.15306034567</v>
       </c>
       <c r="AY2" t="n">
-        <v>31806.67516575943</v>
+        <v>31806.67516575942</v>
       </c>
       <c r="AZ2" t="n">
         <v>32735.05710360176</v>
@@ -828,13 +828,13 @@
         <v>40230.06506465727</v>
       </c>
       <c r="BI2" t="n">
-        <v>41155.99257634705</v>
+        <v>41155.99257634706</v>
       </c>
       <c r="BJ2" t="n">
         <v>42074.87530801022</v>
       </c>
       <c r="BK2" t="n">
-        <v>42985.26219060672</v>
+        <v>42985.26219060673</v>
       </c>
       <c r="BL2" t="n">
         <v>43885.68571787135</v>
@@ -2549,19 +2549,19 @@
         <v>835482586.9509116</v>
       </c>
       <c r="BI11" t="n">
-        <v>828509591.8345453</v>
+        <v>828509591.8345451</v>
       </c>
       <c r="BJ11" t="n">
-        <v>821348136.6399163</v>
+        <v>821348136.6399161</v>
       </c>
       <c r="BK11" t="n">
-        <v>814003866.5551916</v>
+        <v>814003866.5551914</v>
       </c>
       <c r="BL11" t="n">
-        <v>806482555.2447133</v>
+        <v>806482555.2447132</v>
       </c>
       <c r="BM11" t="n">
-        <v>798790096.4903573</v>
+        <v>798790096.4903572</v>
       </c>
     </row>
     <row r="12">
@@ -2620,34 +2620,34 @@
         <v>540628820.50261</v>
       </c>
       <c r="U12" t="n">
-        <v>551864940.7207717</v>
+        <v>551864940.7207716</v>
       </c>
       <c r="V12" t="n">
-        <v>563101060.9389337</v>
+        <v>563101060.9389336</v>
       </c>
       <c r="W12" t="n">
-        <v>574337181.1570958</v>
+        <v>574337181.1570957</v>
       </c>
       <c r="X12" t="n">
-        <v>585573301.3752575</v>
+        <v>585573301.3752574</v>
       </c>
       <c r="Y12" t="n">
-        <v>596809421.5934194</v>
+        <v>596809421.5934193</v>
       </c>
       <c r="Z12" t="n">
-        <v>608186310.7912843</v>
+        <v>608186310.7912842</v>
       </c>
       <c r="AA12" t="n">
-        <v>619563199.9891493</v>
+        <v>619563199.9891492</v>
       </c>
       <c r="AB12" t="n">
-        <v>630940089.1870142</v>
+        <v>630940089.1870141</v>
       </c>
       <c r="AC12" t="n">
-        <v>642316978.3848791</v>
+        <v>642316978.384879</v>
       </c>
       <c r="AD12" t="n">
-        <v>653693867.5827444</v>
+        <v>653693867.5827442</v>
       </c>
       <c r="AE12" t="n">
         <v>665027848.8537953</v>
@@ -2656,103 +2656,103 @@
         <v>676361830.1248463</v>
       </c>
       <c r="AG12" t="n">
-        <v>687695811.3958974</v>
+        <v>687695811.3958975</v>
       </c>
       <c r="AH12" t="n">
-        <v>699029792.6669482</v>
+        <v>699029792.6669483</v>
       </c>
       <c r="AI12" t="n">
-        <v>710363773.9379992</v>
+        <v>710363773.9379995</v>
       </c>
       <c r="AJ12" t="n">
-        <v>721543059.9430301</v>
+        <v>721543059.9430305</v>
       </c>
       <c r="AK12" t="n">
-        <v>732722345.9480613</v>
+        <v>732722345.9480618</v>
       </c>
       <c r="AL12" t="n">
-        <v>743901631.9530921</v>
+        <v>743901631.9530926</v>
       </c>
       <c r="AM12" t="n">
-        <v>755080917.9581232</v>
+        <v>755080917.9581236</v>
       </c>
       <c r="AN12" t="n">
-        <v>766260203.963154</v>
+        <v>766260203.9631543</v>
       </c>
       <c r="AO12" t="n">
-        <v>776945460.7973349</v>
+        <v>776945460.7973353</v>
       </c>
       <c r="AP12" t="n">
-        <v>787630717.6315159</v>
+        <v>787630717.6315162</v>
       </c>
       <c r="AQ12" t="n">
-        <v>798315974.4656968</v>
+        <v>798315974.4656972</v>
       </c>
       <c r="AR12" t="n">
-        <v>809001231.2998776</v>
+        <v>809001231.299878</v>
       </c>
       <c r="AS12" t="n">
-        <v>819686488.1340587</v>
+        <v>819686488.1340591</v>
       </c>
       <c r="AT12" t="n">
-        <v>829543972.0022353</v>
+        <v>829543972.0022358</v>
       </c>
       <c r="AU12" t="n">
-        <v>839197415.0471983</v>
+        <v>839197415.0471988</v>
       </c>
       <c r="AV12" t="n">
-        <v>848636337.6481419</v>
+        <v>848636337.6481423</v>
       </c>
       <c r="AW12" t="n">
-        <v>857850394.4485066</v>
+        <v>857850394.4485071</v>
       </c>
       <c r="AX12" t="n">
-        <v>866829391.9584271</v>
+        <v>866829391.9584275</v>
       </c>
       <c r="AY12" t="n">
-        <v>875563306.1631435</v>
+        <v>875563306.163144</v>
       </c>
       <c r="AZ12" t="n">
-        <v>884042300.0841365</v>
+        <v>884042300.0841371</v>
       </c>
       <c r="BA12" t="n">
-        <v>892256741.240737</v>
+        <v>892256741.2407376</v>
       </c>
       <c r="BB12" t="n">
-        <v>900197218.9608757</v>
+        <v>900197218.9608762</v>
       </c>
       <c r="BC12" t="n">
-        <v>907854561.4905093</v>
+        <v>907854561.4905097</v>
       </c>
       <c r="BD12" t="n">
-        <v>915219852.8521472</v>
+        <v>915219852.8521477</v>
       </c>
       <c r="BE12" t="n">
-        <v>922284449.4038388</v>
+        <v>922284449.4038391</v>
       </c>
       <c r="BF12" t="n">
-        <v>929039996.0509216</v>
+        <v>929039996.0509219</v>
       </c>
       <c r="BG12" t="n">
-        <v>935478442.0638705</v>
+        <v>935478442.0638709</v>
       </c>
       <c r="BH12" t="n">
-        <v>941592056.4567349</v>
+        <v>941592056.4567355</v>
       </c>
       <c r="BI12" t="n">
-        <v>947373442.8818123</v>
+        <v>947373442.8818128</v>
       </c>
       <c r="BJ12" t="n">
-        <v>952815553.9975498</v>
+        <v>952815553.9975504</v>
       </c>
       <c r="BK12" t="n">
-        <v>957911705.2680535</v>
+        <v>957911705.2680541</v>
       </c>
       <c r="BL12" t="n">
-        <v>962655588.1541126</v>
+        <v>962655588.1541132</v>
       </c>
       <c r="BM12" t="n">
-        <v>967041282.6572595</v>
+        <v>967041282.6572601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>